<commit_message>
Change for PLX CMImmunity to be raised to 1.0
Change for PLX CMimmunity to be raised to 1.0 to prevent counter measures effectiveness
</commit_message>
<xml_diff>
--- a/332nd_CapacitySizes.xlsx
+++ b/332nd_CapacitySizes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Modding\332nd_aux_mod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D895EFEC-01F1-4CF2-B5E9-593B13DA90E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B70F45-30D2-4A6E-B249-05F1132B595B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="23310" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -460,7 +460,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>